<commit_message>
Updated validation excel file
</commit_message>
<xml_diff>
--- a/Results_and_scripts_ps/validation_19_06/validation.xlsx
+++ b/Results_and_scripts_ps/validation_19_06/validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>run_20130619T041402</t>
   </si>
   <si>
-    <t>Failed, tolerance problem with ode45</t>
-  </si>
-  <si>
     <t>Error of Ntot at halfway of simulation</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>Error of Vtot at the end of simulation</t>
+  </si>
+  <si>
+    <t>Failed, tolerance problem with ode45. Fixed in later versions.</t>
   </si>
 </sst>
 </file>
@@ -554,11 +554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="39181696"/>
-        <c:axId val="94446720"/>
+        <c:axId val="38460800"/>
+        <c:axId val="105657472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39181696"/>
+        <c:axId val="38460800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,12 +568,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94446720"/>
+        <c:crossAx val="105657472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94446720"/>
+        <c:axId val="105657472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39181696"/>
+        <c:crossAx val="38460800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1002,11 +1002,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94475392"/>
-        <c:axId val="94476928"/>
+        <c:axId val="105682048"/>
+        <c:axId val="105683584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94475392"/>
+        <c:axId val="105682048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,12 +1016,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94476928"/>
+        <c:crossAx val="105683584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94476928"/>
+        <c:axId val="105683584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94475392"/>
+        <c:crossAx val="105682048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1408,7 +1408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -1437,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2424,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O84"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2433,7 @@
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -3348,7 +3348,7 @@
         <v>10</v>
       </c>
       <c r="L32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="N32">
         <f>60</f>

</xml_diff>